<commit_message>
design patterns and small algo updates
</commit_message>
<xml_diff>
--- a/W3/Time Complexities.xlsx
+++ b/W3/Time Complexities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bailey\Desktop\Python_Exercises\W3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bailey\Desktop\L6SD_Python\W3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D92095C-E929-478E-8EA2-183D16105BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125430F1-CCA4-430B-B0BE-49D33093FFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8392790E-AD59-4D4A-A40F-1DCB98F9361D}"/>
+    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{8392790E-AD59-4D4A-A40F-1DCB98F9361D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Bubblesort</t>
   </si>
@@ -96,21 +96,6 @@
   </si>
   <si>
     <t>quick</t>
-  </si>
-  <si>
-    <t>default age</t>
-  </si>
-  <si>
-    <t>default name</t>
-  </si>
-  <si>
-    <t>sorted name</t>
-  </si>
-  <si>
-    <t>reversed name</t>
-  </si>
-  <si>
-    <t>empty</t>
   </si>
   <si>
     <t>default</t>
@@ -133,7 +118,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -209,10 +194,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -554,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A9B5E1-D561-4AB8-8A0B-FBA4F3EA0C00}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,14 +594,12 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G2" s="5"/>
-      <c r="H2" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="H2" s="6"/>
       <c r="K2" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -639,11 +622,9 @@
         <v>0.33100000000000002</v>
       </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="H3" s="6"/>
       <c r="K3" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -663,12 +644,10 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G4" s="5"/>
-      <c r="H4" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -687,12 +666,10 @@
         <v>1E-3</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:18" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -714,9 +691,7 @@
         <v>0.33100000000000002</v>
       </c>
       <c r="G6" s="5"/>
-      <c r="H6" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="H6" s="6"/>
       <c r="M6" t="s">
         <v>15</v>
       </c>
@@ -735,7 +710,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="L7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="M7" s="4">
         <v>8.7387999999999995</v>

</xml_diff>

<commit_message>
pytest done and quicksort improved
</commit_message>
<xml_diff>
--- a/W3/Time Complexities.xlsx
+++ b/W3/Time Complexities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bailey\Desktop\L6SD_Python\W3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125430F1-CCA4-430B-B0BE-49D33093FFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAEA2D2-4CFB-459E-9C1A-89A16D1BB349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{8392790E-AD59-4D4A-A40F-1DCB98F9361D}"/>
+    <workbookView xWindow="8784" yWindow="1188" windowWidth="10992" windowHeight="8964" xr2:uid="{8392790E-AD59-4D4A-A40F-1DCB98F9361D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Bubblesort</t>
   </si>
@@ -69,48 +69,6 @@
   </si>
   <si>
     <t>Duplicate</t>
-  </si>
-  <si>
-    <t>Quick Sort is faster at doing names than numbers</t>
-  </si>
-  <si>
-    <t>Selection Sort is faster at doing numbers (age) than names</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>bubble</t>
-  </si>
-  <si>
-    <t>insert</t>
-  </si>
-  <si>
-    <t>select</t>
-  </si>
-  <si>
-    <t>merge</t>
-  </si>
-  <si>
-    <t>quick</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>Assuming that the only difference between Age and Name is that Age has duplicates</t>
-  </si>
-  <si>
-    <t>Error (max recursion)</t>
-  </si>
-  <si>
-    <t>All times are highly variable, so the numbers here are likely impercise but still provide good comparisons between each sorting method</t>
-  </si>
-  <si>
-    <t>Error (index out of range)</t>
   </si>
 </sst>
 </file>
@@ -537,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A9B5E1-D561-4AB8-8A0B-FBA4F3EA0C00}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,7 +514,7 @@
     <col min="11" max="11" width="36.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -577,84 +535,80 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5">
-        <v>7.6669999999999998</v>
+        <v>2.9860000000000002</v>
       </c>
       <c r="C2" s="5">
-        <v>8.0000000000000002E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D2" s="5">
-        <v>0.57099999999999995</v>
+        <v>0.44</v>
       </c>
       <c r="E2" s="5">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>22</v>
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="F2" s="5">
+        <v>3.161</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="6"/>
-      <c r="K2" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:17" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="5">
-        <v>8.7387999999999995</v>
+        <v>3.9830000000000001</v>
       </c>
       <c r="C3" s="5">
-        <v>5.0000000000000001E-3</v>
+        <v>1.29</v>
       </c>
       <c r="D3" s="5">
-        <v>0.224</v>
+        <v>0.58099999999999996</v>
       </c>
       <c r="E3" s="5">
-        <v>0.12</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="F3" s="5">
-        <v>0.33100000000000002</v>
+        <v>2.3E-2</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="6"/>
-      <c r="K3" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:17" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="5">
-        <v>9.4209999999999994</v>
+        <v>5.0030000000000001</v>
       </c>
       <c r="C4" s="5">
-        <v>4.0000000000000001E-3</v>
+        <v>2.5449999999999999</v>
       </c>
       <c r="D4" s="5">
-        <v>0.40200000000000002</v>
+        <v>0.88</v>
       </c>
       <c r="E4" s="5">
-        <v>0.10299999999999999</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>22</v>
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2.419</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="5">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="C5" s="5">
         <v>0</v>
@@ -663,103 +617,49 @@
         <v>0</v>
       </c>
       <c r="E5" s="5">
-        <v>1E-3</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>24</v>
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:18" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="4">
-        <v>8.7387999999999995</v>
+        <v>2.3860000000000001</v>
       </c>
       <c r="C6" s="4">
-        <v>5.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D6" s="4">
-        <v>0.224</v>
+        <v>0.26</v>
       </c>
       <c r="E6" s="4">
-        <v>0.12</v>
+        <v>3.9E-2</v>
       </c>
       <c r="F6" s="4">
-        <v>0.33100000000000002</v>
+        <v>1.2170000000000001</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="6"/>
-      <c r="M6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O6" t="s">
-        <v>17</v>
-      </c>
-      <c r="P6" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="L7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="4">
-        <v>8.7387999999999995</v>
-      </c>
-      <c r="N7" s="4">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="O7" s="4">
-        <v>0.224</v>
-      </c>
-      <c r="P7" s="4">
-        <v>0.12</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>0.33100000000000002</v>
-      </c>
-      <c r="R7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="M8" s="4">
-        <v>8.2880000000000003</v>
-      </c>
-      <c r="N8" s="4">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="O8" s="4">
-        <v>0.44700000000000001</v>
-      </c>
-      <c r="P8" s="4">
-        <v>0.115</v>
-      </c>
-      <c r="Q8" s="4">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="R8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="M10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="M11" t="s">
-        <v>11</v>
-      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>